<commit_message>
set up electricity base load and activity triggered technologies by duration
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario_Technology_Duration.xlsx
+++ b/data/input_behavior/BehaviorScenario_Technology_Duration.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yus\Documents\code\3E\FLEX\data\input_behavior\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rickm\Documents\Git\Flex\data\input_behavior\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF75530C-07B6-4431-8F1D-B35CFAACF368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4065" yWindow="-17220" windowWidth="24615" windowHeight="13695"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -100,7 +101,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -411,14 +412,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
@@ -444,7 +445,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -455,7 +456,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -466,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -477,7 +478,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -488,7 +489,7 @@
         <v>3</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -499,7 +500,7 @@
         <v>3</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -510,7 +511,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -521,7 +522,7 @@
         <v>3</v>
       </c>
       <c r="C9" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -532,7 +533,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -543,7 +544,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -554,7 +555,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -565,7 +566,7 @@
         <v>3</v>
       </c>
       <c r="C13" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -576,7 +577,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -587,7 +588,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -609,7 +610,7 @@
         <v>3</v>
       </c>
       <c r="C17" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -620,7 +621,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -631,7 +632,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -642,7 +643,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -653,7 +654,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -664,7 +665,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -708,7 +709,7 @@
         <v>3</v>
       </c>
       <c r="C26" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -719,7 +720,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -730,7 +731,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -741,7 +742,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -752,7 +753,7 @@
         <v>3</v>
       </c>
       <c r="C30" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -763,7 +764,7 @@
         <v>3</v>
       </c>
       <c r="C31" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -774,7 +775,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -785,7 +786,7 @@
         <v>3</v>
       </c>
       <c r="C33" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -796,7 +797,7 @@
         <v>3</v>
       </c>
       <c r="C34" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -807,7 +808,7 @@
         <v>3</v>
       </c>
       <c r="C35" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -818,7 +819,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -829,7 +830,7 @@
         <v>3</v>
       </c>
       <c r="C37" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -840,7 +841,7 @@
         <v>3</v>
       </c>
       <c r="C38" s="2">
-        <v>144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -851,7 +852,7 @@
         <v>3</v>
       </c>
       <c r="C39" s="2">
-        <v>144</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -862,7 +863,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="2">
-        <v>144</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -871,15 +872,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="f971c2dd-4979-4752-97a1-eb062e2c22bf" xsi:nil="true"/>
@@ -895,6 +887,15 @@
     </SharedWithUsers>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1103,20 +1104,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{257DA3DA-5CBF-44C8-AF96-57A945D7109F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4123E9A7-AD52-4A33-BBDD-39D9E770116F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="f971c2dd-4979-4752-97a1-eb062e2c22bf"/>
     <ds:schemaRef ds:uri="ed526690-1b82-4476-9598-c0eeafad58f9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{257DA3DA-5CBF-44C8-AF96-57A945D7109F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
technology types removed and duration revised
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario_Technology_Duration.xlsx
+++ b/data/input_behavior/BehaviorScenario_Technology_Duration.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rickm\Documents\Git\Flex\data\input_behavior\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yus\Documents\code\3E\FLEX\data\input_behavior\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF75530C-07B6-4431-8F1D-B35CFAACF368}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="15720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,7 +100,7 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -412,14 +411,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.42578125" customWidth="1"/>
@@ -588,7 +587,7 @@
         <v>3</v>
       </c>
       <c r="C15" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -621,7 +620,7 @@
         <v>3</v>
       </c>
       <c r="C18" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -632,7 +631,7 @@
         <v>3</v>
       </c>
       <c r="C19" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -643,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -654,7 +653,7 @@
         <v>3</v>
       </c>
       <c r="C21" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -665,7 +664,7 @@
         <v>3</v>
       </c>
       <c r="C22" s="2">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -720,7 +719,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -731,7 +730,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -742,7 +741,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="2">
-        <v>1</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -872,33 +871,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="f971c2dd-4979-4752-97a1-eb062e2c22bf" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed526690-1b82-4476-9598-c0eeafad58f9">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <SharedWithUsers xmlns="f971c2dd-4979-4752-97a1-eb062e2c22bf">
-      <UserInfo>
-        <DisplayName>Yu, Songmin</DisplayName>
-        <AccountId>9</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001383FD7952F44C4AA66F138C1496F932" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0f10bb0856646bfda2b94dc29ed0a887">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ed526690-1b82-4476-9598-c0eeafad58f9" xmlns:ns3="f971c2dd-4979-4752-97a1-eb062e2c22bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca21336e7eb6462c50ac4645cdd355ca" ns2:_="" ns3:_="">
     <xsd:import namespace="ed526690-1b82-4476-9598-c0eeafad58f9"/>
@@ -1103,26 +1075,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4123E9A7-AD52-4A33-BBDD-39D9E770116F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f971c2dd-4979-4752-97a1-eb062e2c22bf"/>
-    <ds:schemaRef ds:uri="ed526690-1b82-4476-9598-c0eeafad58f9"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{257DA3DA-5CBF-44C8-AF96-57A945D7109F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="f971c2dd-4979-4752-97a1-eb062e2c22bf" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed526690-1b82-4476-9598-c0eeafad58f9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <SharedWithUsers xmlns="f971c2dd-4979-4752-97a1-eb062e2c22bf">
+      <UserInfo>
+        <DisplayName>Yu, Songmin</DisplayName>
+        <AccountId>9</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A82277C-FB17-4D03-8A51-E0EB9D4B4B52}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1139,4 +1119,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{257DA3DA-5CBF-44C8-AF96-57A945D7109F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4123E9A7-AD52-4A33-BBDD-39D9E770116F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f971c2dd-4979-4752-97a1-eb062e2c22bf"/>
+    <ds:schemaRef ds:uri="ed526690-1b82-4476-9598-c0eeafad58f9"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
consumption removed when outside
</commit_message>
<xml_diff>
--- a/data/input_behavior/BehaviorScenario_Technology_Duration.xlsx
+++ b/data/input_behavior/BehaviorScenario_Technology_Duration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/FLEX/data/input_behavior/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DE559D8-0A33-2D4F-BBFA-BC636E896830}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6967EA29-5E83-8247-85F4-54376C8BE260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1640" yWindow="-20160" windowWidth="10800" windowHeight="18320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-1640" yWindow="-20160" windowWidth="26280" windowHeight="18760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="288" zoomScaleNormal="288" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -854,6 +854,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x0101001383FD7952F44C4AA66F138C1496F932" ma:contentTypeVersion="10" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="0f10bb0856646bfda2b94dc29ed0a887">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="ed526690-1b82-4476-9598-c0eeafad58f9" xmlns:ns3="f971c2dd-4979-4752-97a1-eb062e2c22bf" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ca21336e7eb6462c50ac4645cdd355ca" ns2:_="" ns3:_="">
     <xsd:import namespace="ed526690-1b82-4476-9598-c0eeafad58f9"/>
@@ -1058,15 +1067,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1086,6 +1086,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{257DA3DA-5CBF-44C8-AF96-57A945D7109F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1A82277C-FB17-4D03-8A51-E0EB9D4B4B52}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1104,14 +1112,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{257DA3DA-5CBF-44C8-AF96-57A945D7109F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4123E9A7-AD52-4A33-BBDD-39D9E770116F}">
   <ds:schemaRefs>

</xml_diff>